<commit_message>
customerslist added in database
</commit_message>
<xml_diff>
--- a/src/Prize List.xlsx
+++ b/src/Prize List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khalil Gulraiz\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Lucky Draw\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,15 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>handle</t>
+    <t>numbers</t>
   </si>
 </sst>
 </file>
@@ -350,23 +344,268 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:A43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A43" si="0">A3+1</f>
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f>A30+1</f>
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>1139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>